<commit_message>
Update 17-3-2020, rivm csv format changed so I updated test.py. To-do: create output with 2 new columns
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W356"/>
+  <dimension ref="A1:X356"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +482,11 @@
           <t>16-03-2020</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>17-03-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -557,6 +562,9 @@
       <c r="W2" t="n">
         <v>14</v>
       </c>
+      <c r="X2" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -632,6 +640,9 @@
       <c r="W3" t="n">
         <v>20</v>
       </c>
+      <c r="X3" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -707,6 +718,9 @@
       <c r="W4" t="n">
         <v>0</v>
       </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -782,6 +796,9 @@
       <c r="W5" t="n">
         <v>3</v>
       </c>
+      <c r="X5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -857,6 +874,9 @@
       <c r="W6" t="n">
         <v>0</v>
       </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -932,6 +952,9 @@
       <c r="W7" t="n">
         <v>0</v>
       </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1007,6 +1030,9 @@
       <c r="W8" t="n">
         <v>0</v>
       </c>
+      <c r="X8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1082,6 +1108,9 @@
       <c r="W9" t="n">
         <v>2</v>
       </c>
+      <c r="X9" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1157,6 +1186,9 @@
       <c r="W10" t="n">
         <v>2</v>
       </c>
+      <c r="X10" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1232,6 +1264,9 @@
       <c r="W11" t="n">
         <v>1</v>
       </c>
+      <c r="X11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1307,6 +1342,9 @@
       <c r="W12" t="n">
         <v>3</v>
       </c>
+      <c r="X12" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1382,6 +1420,9 @@
       <c r="W13" t="n">
         <v>6</v>
       </c>
+      <c r="X13" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1457,6 +1498,9 @@
       <c r="W14" t="n">
         <v>2</v>
       </c>
+      <c r="X14" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1532,6 +1576,9 @@
       <c r="W15" t="n">
         <v>12</v>
       </c>
+      <c r="X15" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1607,6 +1654,9 @@
       <c r="W16" t="n">
         <v>0</v>
       </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1682,6 +1732,9 @@
       <c r="W17" t="n">
         <v>18</v>
       </c>
+      <c r="X17" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1757,6 +1810,9 @@
       <c r="W18" t="n">
         <v>4</v>
       </c>
+      <c r="X18" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1832,6 +1888,9 @@
       <c r="W19" t="n">
         <v>39</v>
       </c>
+      <c r="X19" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1907,6 +1966,9 @@
       <c r="W20" t="n">
         <v>7</v>
       </c>
+      <c r="X20" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1982,6 +2044,9 @@
       <c r="W21" t="n">
         <v>0</v>
       </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2057,6 +2122,9 @@
       <c r="W22" t="n">
         <v>7</v>
       </c>
+      <c r="X22" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2132,6 +2200,9 @@
       <c r="W23" t="n">
         <v>0</v>
       </c>
+      <c r="X23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2207,6 +2278,9 @@
       <c r="W24" t="n">
         <v>1</v>
       </c>
+      <c r="X24" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2282,6 +2356,9 @@
       <c r="W25" t="n">
         <v>0</v>
       </c>
+      <c r="X25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2357,6 +2434,9 @@
       <c r="W26" t="n">
         <v>0</v>
       </c>
+      <c r="X26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2432,6 +2512,9 @@
       <c r="W27" t="n">
         <v>3</v>
       </c>
+      <c r="X27" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2507,6 +2590,9 @@
       <c r="W28" t="n">
         <v>3</v>
       </c>
+      <c r="X28" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2582,6 +2668,9 @@
       <c r="W29" t="n">
         <v>3</v>
       </c>
+      <c r="X29" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2657,6 +2746,9 @@
       <c r="W30" t="n">
         <v>13</v>
       </c>
+      <c r="X30" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2732,6 +2824,9 @@
       <c r="W31" t="n">
         <v>0</v>
       </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2807,6 +2902,9 @@
       <c r="W32" t="n">
         <v>0</v>
       </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2882,6 +2980,9 @@
       <c r="W33" t="n">
         <v>10</v>
       </c>
+      <c r="X33" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2957,6 +3058,9 @@
       <c r="W34" t="n">
         <v>1</v>
       </c>
+      <c r="X34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3032,6 +3136,9 @@
       <c r="W35" t="n">
         <v>0</v>
       </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3107,6 +3214,9 @@
       <c r="W36" t="n">
         <v>1</v>
       </c>
+      <c r="X36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3182,6 +3292,9 @@
       <c r="W37" t="n">
         <v>4</v>
       </c>
+      <c r="X37" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3257,6 +3370,9 @@
       <c r="W38" t="n">
         <v>0</v>
       </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3332,6 +3448,9 @@
       <c r="W39" t="n">
         <v>19</v>
       </c>
+      <c r="X39" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3407,6 +3526,9 @@
       <c r="W40" t="n">
         <v>4</v>
       </c>
+      <c r="X40" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3482,6 +3604,9 @@
       <c r="W41" t="n">
         <v>5</v>
       </c>
+      <c r="X41" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3557,6 +3682,9 @@
       <c r="W42" t="n">
         <v>5</v>
       </c>
+      <c r="X42" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3632,6 +3760,9 @@
       <c r="W43" t="n">
         <v>1</v>
       </c>
+      <c r="X43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -3707,6 +3838,9 @@
       <c r="W44" t="n">
         <v>1</v>
       </c>
+      <c r="X44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -3782,6 +3916,9 @@
       <c r="W45" t="n">
         <v>1</v>
       </c>
+      <c r="X45" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -3857,6 +3994,9 @@
       <c r="W46" t="n">
         <v>1</v>
       </c>
+      <c r="X46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -3932,6 +4072,9 @@
       <c r="W47" t="n">
         <v>14</v>
       </c>
+      <c r="X47" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -4007,6 +4150,9 @@
       <c r="W48" t="n">
         <v>0</v>
       </c>
+      <c r="X48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -4082,6 +4228,9 @@
       <c r="W49" t="n">
         <v>3</v>
       </c>
+      <c r="X49" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -4157,6 +4306,9 @@
       <c r="W50" t="n">
         <v>2</v>
       </c>
+      <c r="X50" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -4232,6 +4384,9 @@
       <c r="W51" t="n">
         <v>1</v>
       </c>
+      <c r="X51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -4307,6 +4462,9 @@
       <c r="W52" t="n">
         <v>3</v>
       </c>
+      <c r="X52" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -4382,6 +4540,9 @@
       <c r="W53" t="n">
         <v>86</v>
       </c>
+      <c r="X53" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -4457,6 +4618,9 @@
       <c r="W54" t="n">
         <v>0</v>
       </c>
+      <c r="X54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -4532,6 +4696,9 @@
       <c r="W55" t="n">
         <v>2</v>
       </c>
+      <c r="X55" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -4607,6 +4774,9 @@
       <c r="W56" t="n">
         <v>0</v>
       </c>
+      <c r="X56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -4682,6 +4852,9 @@
       <c r="W57" t="n">
         <v>0</v>
       </c>
+      <c r="X57" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -4757,6 +4930,9 @@
       <c r="W58" t="n">
         <v>0</v>
       </c>
+      <c r="X58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -4832,6 +5008,9 @@
       <c r="W59" t="n">
         <v>0</v>
       </c>
+      <c r="X59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -4907,6 +5086,9 @@
       <c r="W60" t="n">
         <v>4</v>
       </c>
+      <c r="X60" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -4982,6 +5164,9 @@
       <c r="W61" t="n">
         <v>0</v>
       </c>
+      <c r="X61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -5057,6 +5242,9 @@
       <c r="W62" t="n">
         <v>5</v>
       </c>
+      <c r="X62" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -5132,6 +5320,9 @@
       <c r="W63" t="n">
         <v>11</v>
       </c>
+      <c r="X63" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -5207,6 +5398,9 @@
       <c r="W64" t="n">
         <v>2</v>
       </c>
+      <c r="X64" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -5282,6 +5476,9 @@
       <c r="W65" t="n">
         <v>2</v>
       </c>
+      <c r="X65" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -5357,6 +5554,9 @@
       <c r="W66" t="n">
         <v>2</v>
       </c>
+      <c r="X66" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -5432,6 +5632,9 @@
       <c r="W67" t="n">
         <v>1</v>
       </c>
+      <c r="X67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -5507,6 +5710,9 @@
       <c r="W68" t="n">
         <v>0</v>
       </c>
+      <c r="X68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -5582,6 +5788,9 @@
       <c r="W69" t="n">
         <v>13</v>
       </c>
+      <c r="X69" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -5657,6 +5866,9 @@
       <c r="W70" t="n">
         <v>3</v>
       </c>
+      <c r="X70" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -5732,6 +5944,9 @@
       <c r="W71" t="n">
         <v>2</v>
       </c>
+      <c r="X71" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -5807,6 +6022,9 @@
       <c r="W72" t="n">
         <v>1</v>
       </c>
+      <c r="X72" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -5882,6 +6100,9 @@
       <c r="W73" t="n">
         <v>2</v>
       </c>
+      <c r="X73" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -5957,6 +6178,9 @@
       <c r="W74" t="n">
         <v>0</v>
       </c>
+      <c r="X74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -6032,6 +6256,9 @@
       <c r="W75" t="n">
         <v>1</v>
       </c>
+      <c r="X75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -6107,6 +6334,9 @@
       <c r="W76" t="n">
         <v>5</v>
       </c>
+      <c r="X76" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -6182,6 +6412,9 @@
       <c r="W77" t="n">
         <v>2</v>
       </c>
+      <c r="X77" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -6257,6 +6490,9 @@
       <c r="W78" t="n">
         <v>2</v>
       </c>
+      <c r="X78" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -6332,6 +6568,9 @@
       <c r="W79" t="n">
         <v>5</v>
       </c>
+      <c r="X79" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -6407,6 +6646,9 @@
       <c r="W80" t="n">
         <v>1</v>
       </c>
+      <c r="X80" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -6482,6 +6724,9 @@
       <c r="W81" t="n">
         <v>0</v>
       </c>
+      <c r="X81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -6557,6 +6802,9 @@
       <c r="W82" t="n">
         <v>5</v>
       </c>
+      <c r="X82" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -6632,6 +6880,9 @@
       <c r="W83" t="n">
         <v>1</v>
       </c>
+      <c r="X83" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -6707,6 +6958,9 @@
       <c r="W84" t="n">
         <v>0</v>
       </c>
+      <c r="X84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -6782,6 +7036,9 @@
       <c r="W85" t="n">
         <v>7</v>
       </c>
+      <c r="X85" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -6857,6 +7114,9 @@
       <c r="W86" t="n">
         <v>7</v>
       </c>
+      <c r="X86" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -6932,6 +7192,9 @@
       <c r="W87" t="n">
         <v>5</v>
       </c>
+      <c r="X87" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -7007,6 +7270,9 @@
       <c r="W88" t="n">
         <v>1</v>
       </c>
+      <c r="X88" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -7082,6 +7348,9 @@
       <c r="W89" t="n">
         <v>0</v>
       </c>
+      <c r="X89" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -7157,6 +7426,9 @@
       <c r="W90" t="n">
         <v>0</v>
       </c>
+      <c r="X90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -7232,6 +7504,9 @@
       <c r="W91" t="n">
         <v>2</v>
       </c>
+      <c r="X91" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -7307,6 +7582,9 @@
       <c r="W92" t="n">
         <v>0</v>
       </c>
+      <c r="X92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -7382,6 +7660,9 @@
       <c r="W93" t="n">
         <v>2</v>
       </c>
+      <c r="X93" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -7457,6 +7738,9 @@
       <c r="W94" t="n">
         <v>4</v>
       </c>
+      <c r="X94" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -7532,6 +7816,9 @@
       <c r="W95" t="n">
         <v>21</v>
       </c>
+      <c r="X95" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -7607,6 +7894,9 @@
       <c r="W96" t="n">
         <v>1</v>
       </c>
+      <c r="X96" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -7682,6 +7972,9 @@
       <c r="W97" t="n">
         <v>1</v>
       </c>
+      <c r="X97" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -7757,6 +8050,9 @@
       <c r="W98" t="n">
         <v>1</v>
       </c>
+      <c r="X98" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -7832,6 +8128,9 @@
       <c r="W99" t="n">
         <v>3</v>
       </c>
+      <c r="X99" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -7907,6 +8206,9 @@
       <c r="W100" t="n">
         <v>2</v>
       </c>
+      <c r="X100" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -7982,6 +8284,9 @@
       <c r="W101" t="n">
         <v>8</v>
       </c>
+      <c r="X101" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -8057,6 +8362,9 @@
       <c r="W102" t="n">
         <v>10</v>
       </c>
+      <c r="X102" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -8132,6 +8440,9 @@
       <c r="W103" t="n">
         <v>3</v>
       </c>
+      <c r="X103" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -8207,6 +8518,9 @@
       <c r="W104" t="n">
         <v>3</v>
       </c>
+      <c r="X104" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -8282,6 +8596,9 @@
       <c r="W105" t="n">
         <v>20</v>
       </c>
+      <c r="X105" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -8357,6 +8674,9 @@
       <c r="W106" t="n">
         <v>1</v>
       </c>
+      <c r="X106" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -8432,6 +8752,9 @@
       <c r="W107" t="n">
         <v>1</v>
       </c>
+      <c r="X107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -8507,6 +8830,9 @@
       <c r="W108" t="n">
         <v>4</v>
       </c>
+      <c r="X108" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -8582,6 +8908,9 @@
       <c r="W109" t="n">
         <v>2</v>
       </c>
+      <c r="X109" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -8657,6 +8986,9 @@
       <c r="W110" t="n">
         <v>9</v>
       </c>
+      <c r="X110" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -8732,6 +9064,9 @@
       <c r="W111" t="n">
         <v>4</v>
       </c>
+      <c r="X111" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -8807,6 +9142,9 @@
       <c r="W112" t="n">
         <v>0</v>
       </c>
+      <c r="X112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -8882,6 +9220,9 @@
       <c r="W113" t="n">
         <v>4</v>
       </c>
+      <c r="X113" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -8957,6 +9298,9 @@
       <c r="W114" t="n">
         <v>0</v>
       </c>
+      <c r="X114" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -9032,6 +9376,9 @@
       <c r="W115" t="n">
         <v>7</v>
       </c>
+      <c r="X115" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -9107,6 +9454,9 @@
       <c r="W116" t="n">
         <v>2</v>
       </c>
+      <c r="X116" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -9182,6 +9532,9 @@
       <c r="W117" t="n">
         <v>1</v>
       </c>
+      <c r="X117" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -9257,6 +9610,9 @@
       <c r="W118" t="n">
         <v>7</v>
       </c>
+      <c r="X118" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -9332,6 +9688,9 @@
       <c r="W119" t="n">
         <v>6</v>
       </c>
+      <c r="X119" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -9407,6 +9766,9 @@
       <c r="W120" t="n">
         <v>2</v>
       </c>
+      <c r="X120" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -9482,6 +9844,9 @@
       <c r="W121" t="n">
         <v>2</v>
       </c>
+      <c r="X121" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -9557,6 +9922,9 @@
       <c r="W122" t="n">
         <v>0</v>
       </c>
+      <c r="X122" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -9632,6 +10000,9 @@
       <c r="W123" t="n">
         <v>4</v>
       </c>
+      <c r="X123" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -9707,6 +10078,9 @@
       <c r="W124" t="n">
         <v>5</v>
       </c>
+      <c r="X124" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -9782,6 +10156,9 @@
       <c r="W125" t="n">
         <v>1</v>
       </c>
+      <c r="X125" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -9857,6 +10234,9 @@
       <c r="W126" t="n">
         <v>0</v>
       </c>
+      <c r="X126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -9932,6 +10312,9 @@
       <c r="W127" t="n">
         <v>2</v>
       </c>
+      <c r="X127" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -10007,6 +10390,9 @@
       <c r="W128" t="n">
         <v>5</v>
       </c>
+      <c r="X128" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -10082,6 +10468,9 @@
       <c r="W129" t="n">
         <v>2</v>
       </c>
+      <c r="X129" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -10157,6 +10546,9 @@
       <c r="W130" t="n">
         <v>0</v>
       </c>
+      <c r="X130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -10232,6 +10624,9 @@
       <c r="W131" t="n">
         <v>1</v>
       </c>
+      <c r="X131" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -10307,6 +10702,9 @@
       <c r="W132" t="n">
         <v>6</v>
       </c>
+      <c r="X132" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -10382,6 +10780,9 @@
       <c r="W133" t="n">
         <v>2</v>
       </c>
+      <c r="X133" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -10457,6 +10858,9 @@
       <c r="W134" t="n">
         <v>3</v>
       </c>
+      <c r="X134" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -10532,6 +10936,9 @@
       <c r="W135" t="n">
         <v>2</v>
       </c>
+      <c r="X135" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -10607,6 +11014,9 @@
       <c r="W136" t="n">
         <v>1</v>
       </c>
+      <c r="X136" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -10682,6 +11092,9 @@
       <c r="W137" t="n">
         <v>17</v>
       </c>
+      <c r="X137" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -10757,6 +11170,9 @@
       <c r="W138" t="n">
         <v>0</v>
       </c>
+      <c r="X138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -10832,6 +11248,9 @@
       <c r="W139" t="n">
         <v>3</v>
       </c>
+      <c r="X139" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -10907,6 +11326,9 @@
       <c r="W140" t="n">
         <v>0</v>
       </c>
+      <c r="X140" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -10982,6 +11404,9 @@
       <c r="W141" t="n">
         <v>2</v>
       </c>
+      <c r="X141" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -11057,6 +11482,9 @@
       <c r="W142" t="n">
         <v>4</v>
       </c>
+      <c r="X142" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -11132,6 +11560,9 @@
       <c r="W143" t="n">
         <v>0</v>
       </c>
+      <c r="X143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -11207,6 +11638,9 @@
       <c r="W144" t="n">
         <v>4</v>
       </c>
+      <c r="X144" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -11282,6 +11716,9 @@
       <c r="W145" t="n">
         <v>0</v>
       </c>
+      <c r="X145" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -11357,6 +11794,9 @@
       <c r="W146" t="n">
         <v>4</v>
       </c>
+      <c r="X146" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -11432,6 +11872,9 @@
       <c r="W147" t="n">
         <v>1</v>
       </c>
+      <c r="X147" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -11507,6 +11950,9 @@
       <c r="W148" t="n">
         <v>0</v>
       </c>
+      <c r="X148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -11582,6 +12028,9 @@
       <c r="W149" t="n">
         <v>2</v>
       </c>
+      <c r="X149" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -11657,6 +12106,9 @@
       <c r="W150" t="n">
         <v>1</v>
       </c>
+      <c r="X150" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -11732,6 +12184,9 @@
       <c r="W151" t="n">
         <v>5</v>
       </c>
+      <c r="X151" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -11807,6 +12262,9 @@
       <c r="W152" t="n">
         <v>13</v>
       </c>
+      <c r="X152" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -11882,6 +12340,9 @@
       <c r="W153" t="n">
         <v>1</v>
       </c>
+      <c r="X153" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -11957,6 +12418,9 @@
       <c r="W154" t="n">
         <v>0</v>
       </c>
+      <c r="X154" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -12032,6 +12496,9 @@
       <c r="W155" t="n">
         <v>4</v>
       </c>
+      <c r="X155" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -12107,6 +12574,9 @@
       <c r="W156" t="n">
         <v>0</v>
       </c>
+      <c r="X156" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -12182,6 +12652,9 @@
       <c r="W157" t="n">
         <v>0</v>
       </c>
+      <c r="X157" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -12257,6 +12730,9 @@
       <c r="W158" t="n">
         <v>0</v>
       </c>
+      <c r="X158" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -12332,6 +12808,9 @@
       <c r="W159" t="n">
         <v>1</v>
       </c>
+      <c r="X159" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -12407,6 +12886,9 @@
       <c r="W160" t="n">
         <v>2</v>
       </c>
+      <c r="X160" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -12482,6 +12964,9 @@
       <c r="W161" t="n">
         <v>1</v>
       </c>
+      <c r="X161" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -12557,6 +13042,9 @@
       <c r="W162" t="n">
         <v>1</v>
       </c>
+      <c r="X162" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -12632,6 +13120,9 @@
       <c r="W163" t="n">
         <v>4</v>
       </c>
+      <c r="X163" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -12707,6 +13198,9 @@
       <c r="W164" t="n">
         <v>1</v>
       </c>
+      <c r="X164" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -12782,6 +13276,9 @@
       <c r="W165" t="n">
         <v>10</v>
       </c>
+      <c r="X165" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -12857,6 +13354,9 @@
       <c r="W166" t="n">
         <v>4</v>
       </c>
+      <c r="X166" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -12932,6 +13432,9 @@
       <c r="W167" t="n">
         <v>3</v>
       </c>
+      <c r="X167" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -13007,6 +13510,9 @@
       <c r="W168" t="n">
         <v>4</v>
       </c>
+      <c r="X168" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -13082,6 +13588,9 @@
       <c r="W169" t="n">
         <v>5</v>
       </c>
+      <c r="X169" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -13157,6 +13666,9 @@
       <c r="W170" t="n">
         <v>0</v>
       </c>
+      <c r="X170" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -13232,6 +13744,9 @@
       <c r="W171" t="n">
         <v>2</v>
       </c>
+      <c r="X171" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -13307,6 +13822,9 @@
       <c r="W172" t="n">
         <v>8</v>
       </c>
+      <c r="X172" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -13382,6 +13900,9 @@
       <c r="W173" t="n">
         <v>1</v>
       </c>
+      <c r="X173" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -13457,6 +13978,9 @@
       <c r="W174" t="n">
         <v>4</v>
       </c>
+      <c r="X174" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -13532,6 +14056,9 @@
       <c r="W175" t="n">
         <v>8</v>
       </c>
+      <c r="X175" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -13607,6 +14134,9 @@
       <c r="W176" t="n">
         <v>7</v>
       </c>
+      <c r="X176" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -13682,6 +14212,9 @@
       <c r="W177" t="n">
         <v>1</v>
       </c>
+      <c r="X177" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -13757,6 +14290,9 @@
       <c r="W178" t="n">
         <v>3</v>
       </c>
+      <c r="X178" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -13832,6 +14368,9 @@
       <c r="W179" t="n">
         <v>0</v>
       </c>
+      <c r="X179" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -13907,6 +14446,9 @@
       <c r="W180" t="n">
         <v>0</v>
       </c>
+      <c r="X180" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -13982,6 +14524,9 @@
       <c r="W181" t="n">
         <v>7</v>
       </c>
+      <c r="X181" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -14057,6 +14602,9 @@
       <c r="W182" t="n">
         <v>1</v>
       </c>
+      <c r="X182" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -14132,6 +14680,9 @@
       <c r="W183" t="n">
         <v>0</v>
       </c>
+      <c r="X183" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -14207,6 +14758,9 @@
       <c r="W184" t="n">
         <v>0</v>
       </c>
+      <c r="X184" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -14282,6 +14836,9 @@
       <c r="W185" t="n">
         <v>0</v>
       </c>
+      <c r="X185" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -14357,6 +14914,9 @@
       <c r="W186" t="n">
         <v>2</v>
       </c>
+      <c r="X186" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -14432,6 +14992,9 @@
       <c r="W187" t="n">
         <v>1</v>
       </c>
+      <c r="X187" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -14507,6 +15070,9 @@
       <c r="W188" t="n">
         <v>24</v>
       </c>
+      <c r="X188" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -14582,6 +15148,9 @@
       <c r="W189" t="n">
         <v>0</v>
       </c>
+      <c r="X189" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -14657,6 +15226,9 @@
       <c r="W190" t="n">
         <v>1</v>
       </c>
+      <c r="X190" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -14732,6 +15304,9 @@
       <c r="W191" t="n">
         <v>42</v>
       </c>
+      <c r="X191" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -14807,6 +15382,9 @@
       <c r="W192" t="n">
         <v>0</v>
       </c>
+      <c r="X192" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -14882,6 +15460,9 @@
       <c r="W193" t="n">
         <v>1</v>
       </c>
+      <c r="X193" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -14957,6 +15538,9 @@
       <c r="W194" t="n">
         <v>0</v>
       </c>
+      <c r="X194" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -15032,6 +15616,9 @@
       <c r="W195" t="n">
         <v>0</v>
       </c>
+      <c r="X195" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -15107,6 +15694,9 @@
       <c r="W196" t="n">
         <v>1</v>
       </c>
+      <c r="X196" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -15182,6 +15772,9 @@
       <c r="W197" t="n">
         <v>1</v>
       </c>
+      <c r="X197" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -15257,6 +15850,9 @@
       <c r="W198" t="n">
         <v>1</v>
       </c>
+      <c r="X198" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -15332,6 +15928,9 @@
       <c r="W199" t="n">
         <v>2</v>
       </c>
+      <c r="X199" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -15407,6 +16006,9 @@
       <c r="W200" t="n">
         <v>0</v>
       </c>
+      <c r="X200" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -15482,6 +16084,9 @@
       <c r="W201" t="n">
         <v>0</v>
       </c>
+      <c r="X201" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -15557,6 +16162,9 @@
       <c r="W202" t="n">
         <v>0</v>
       </c>
+      <c r="X202" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -15632,6 +16240,9 @@
       <c r="W203" t="n">
         <v>4</v>
       </c>
+      <c r="X203" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -15707,6 +16318,9 @@
       <c r="W204" t="n">
         <v>3</v>
       </c>
+      <c r="X204" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -15782,6 +16396,9 @@
       <c r="W205" t="n">
         <v>1</v>
       </c>
+      <c r="X205" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -15857,6 +16474,9 @@
       <c r="W206" t="n">
         <v>1</v>
       </c>
+      <c r="X206" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -15932,6 +16552,9 @@
       <c r="W207" t="n">
         <v>1</v>
       </c>
+      <c r="X207" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -16007,6 +16630,9 @@
       <c r="W208" t="n">
         <v>17</v>
       </c>
+      <c r="X208" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -16082,6 +16708,9 @@
       <c r="W209" t="n">
         <v>1</v>
       </c>
+      <c r="X209" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -16157,6 +16786,9 @@
       <c r="W210" t="n">
         <v>0</v>
       </c>
+      <c r="X210" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -16232,6 +16864,9 @@
       <c r="W211" t="n">
         <v>0</v>
       </c>
+      <c r="X211" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -16307,6 +16942,9 @@
       <c r="W212" t="n">
         <v>1</v>
       </c>
+      <c r="X212" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -16382,6 +17020,9 @@
       <c r="W213" t="n">
         <v>2</v>
       </c>
+      <c r="X213" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -16457,6 +17098,9 @@
       <c r="W214" t="n">
         <v>2</v>
       </c>
+      <c r="X214" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -16532,6 +17176,9 @@
       <c r="W215" t="n">
         <v>1</v>
       </c>
+      <c r="X215" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -16607,6 +17254,9 @@
       <c r="W216" t="n">
         <v>2</v>
       </c>
+      <c r="X216" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -16682,6 +17332,9 @@
       <c r="W217" t="n">
         <v>4</v>
       </c>
+      <c r="X217" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -16757,6 +17410,9 @@
       <c r="W218" t="n">
         <v>1</v>
       </c>
+      <c r="X218" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -16832,6 +17488,9 @@
       <c r="W219" t="n">
         <v>9</v>
       </c>
+      <c r="X219" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -16907,6 +17566,9 @@
       <c r="W220" t="n">
         <v>0</v>
       </c>
+      <c r="X220" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -16982,6 +17644,9 @@
       <c r="W221" t="n">
         <v>2</v>
       </c>
+      <c r="X221" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -17057,6 +17722,9 @@
       <c r="W222" t="n">
         <v>1</v>
       </c>
+      <c r="X222" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -17132,6 +17800,9 @@
       <c r="W223" t="n">
         <v>0</v>
       </c>
+      <c r="X223" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -17207,6 +17878,9 @@
       <c r="W224" t="n">
         <v>1</v>
       </c>
+      <c r="X224" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -17282,6 +17956,9 @@
       <c r="W225" t="n">
         <v>0</v>
       </c>
+      <c r="X225" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -17357,6 +18034,9 @@
       <c r="W226" t="n">
         <v>6</v>
       </c>
+      <c r="X226" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -17432,6 +18112,9 @@
       <c r="W227" t="n">
         <v>0</v>
       </c>
+      <c r="X227" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -17507,6 +18190,9 @@
       <c r="W228" t="n">
         <v>0</v>
       </c>
+      <c r="X228" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -17582,6 +18268,9 @@
       <c r="W229" t="n">
         <v>0</v>
       </c>
+      <c r="X229" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -17657,6 +18346,9 @@
       <c r="W230" t="n">
         <v>2</v>
       </c>
+      <c r="X230" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -17732,6 +18424,9 @@
       <c r="W231" t="n">
         <v>11</v>
       </c>
+      <c r="X231" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -17807,6 +18502,9 @@
       <c r="W232" t="n">
         <v>1</v>
       </c>
+      <c r="X232" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -17882,6 +18580,9 @@
       <c r="W233" t="n">
         <v>0</v>
       </c>
+      <c r="X233" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -17957,6 +18658,9 @@
       <c r="W234" t="n">
         <v>1</v>
       </c>
+      <c r="X234" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -18032,6 +18736,9 @@
       <c r="W235" t="n">
         <v>8</v>
       </c>
+      <c r="X235" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -18107,6 +18814,9 @@
       <c r="W236" t="n">
         <v>0</v>
       </c>
+      <c r="X236" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -18182,6 +18892,9 @@
       <c r="W237" t="n">
         <v>19</v>
       </c>
+      <c r="X237" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -18257,6 +18970,9 @@
       <c r="W238" t="n">
         <v>1</v>
       </c>
+      <c r="X238" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -18332,6 +19048,9 @@
       <c r="W239" t="n">
         <v>8</v>
       </c>
+      <c r="X239" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -18407,6 +19126,9 @@
       <c r="W240" t="n">
         <v>2</v>
       </c>
+      <c r="X240" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -18482,6 +19204,9 @@
       <c r="W241" t="n">
         <v>2</v>
       </c>
+      <c r="X241" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -18557,6 +19282,9 @@
       <c r="W242" t="n">
         <v>2</v>
       </c>
+      <c r="X242" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -18632,6 +19360,9 @@
       <c r="W243" t="n">
         <v>2</v>
       </c>
+      <c r="X243" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -18707,6 +19438,9 @@
       <c r="W244" t="n">
         <v>8</v>
       </c>
+      <c r="X244" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -18782,6 +19516,9 @@
       <c r="W245" t="n">
         <v>0</v>
       </c>
+      <c r="X245" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -18857,6 +19594,9 @@
       <c r="W246" t="n">
         <v>0</v>
       </c>
+      <c r="X246" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -18932,6 +19672,9 @@
       <c r="W247" t="n">
         <v>1</v>
       </c>
+      <c r="X247" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -19007,6 +19750,9 @@
       <c r="W248" t="n">
         <v>0</v>
       </c>
+      <c r="X248" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -19082,6 +19828,9 @@
       <c r="W249" t="n">
         <v>1</v>
       </c>
+      <c r="X249" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -19157,6 +19906,9 @@
       <c r="W250" t="n">
         <v>0</v>
       </c>
+      <c r="X250" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -19232,6 +19984,9 @@
       <c r="W251" t="n">
         <v>1</v>
       </c>
+      <c r="X251" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -19307,6 +20062,9 @@
       <c r="W252" t="n">
         <v>0</v>
       </c>
+      <c r="X252" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -19382,6 +20140,9 @@
       <c r="W253" t="n">
         <v>2</v>
       </c>
+      <c r="X253" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -19457,6 +20218,9 @@
       <c r="W254" t="n">
         <v>6</v>
       </c>
+      <c r="X254" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -19532,6 +20296,9 @@
       <c r="W255" t="n">
         <v>30</v>
       </c>
+      <c r="X255" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -19607,6 +20374,9 @@
       <c r="W256" t="n">
         <v>1</v>
       </c>
+      <c r="X256" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -19682,6 +20452,9 @@
       <c r="W257" t="n">
         <v>1</v>
       </c>
+      <c r="X257" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -19757,6 +20530,9 @@
       <c r="W258" t="n">
         <v>4</v>
       </c>
+      <c r="X258" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -19832,6 +20608,9 @@
       <c r="W259" t="n">
         <v>0</v>
       </c>
+      <c r="X259" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -19907,6 +20686,9 @@
       <c r="W260" t="n">
         <v>1</v>
       </c>
+      <c r="X260" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -19982,6 +20764,9 @@
       <c r="W261" t="n">
         <v>0</v>
       </c>
+      <c r="X261" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -20057,6 +20842,9 @@
       <c r="W262" t="n">
         <v>2</v>
       </c>
+      <c r="X262" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -20132,6 +20920,9 @@
       <c r="W263" t="n">
         <v>3</v>
       </c>
+      <c r="X263" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -20207,6 +20998,9 @@
       <c r="W264" t="n">
         <v>3</v>
       </c>
+      <c r="X264" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -20282,6 +21076,9 @@
       <c r="W265" t="n">
         <v>8</v>
       </c>
+      <c r="X265" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -20357,6 +21154,9 @@
       <c r="W266" t="n">
         <v>38</v>
       </c>
+      <c r="X266" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -20432,6 +21232,9 @@
       <c r="W267" t="n">
         <v>0</v>
       </c>
+      <c r="X267" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -20507,6 +21310,9 @@
       <c r="W268" t="n">
         <v>2</v>
       </c>
+      <c r="X268" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -20582,6 +21388,9 @@
       <c r="W269" t="n">
         <v>3</v>
       </c>
+      <c r="X269" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -20657,6 +21466,9 @@
       <c r="W270" t="n">
         <v>10</v>
       </c>
+      <c r="X270" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -20732,6 +21544,9 @@
       <c r="W271" t="n">
         <v>1</v>
       </c>
+      <c r="X271" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -20807,6 +21622,9 @@
       <c r="W272" t="n">
         <v>4</v>
       </c>
+      <c r="X272" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -20882,6 +21700,9 @@
       <c r="W273" t="n">
         <v>0</v>
       </c>
+      <c r="X273" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -20957,6 +21778,9 @@
       <c r="W274" t="n">
         <v>1</v>
       </c>
+      <c r="X274" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -21032,6 +21856,9 @@
       <c r="W275" t="n">
         <v>1</v>
       </c>
+      <c r="X275" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -21107,6 +21934,9 @@
       <c r="W276" t="n">
         <v>2</v>
       </c>
+      <c r="X276" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -21182,6 +22012,9 @@
       <c r="W277" t="n">
         <v>0</v>
       </c>
+      <c r="X277" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -21257,6 +22090,9 @@
       <c r="W278" t="n">
         <v>3</v>
       </c>
+      <c r="X278" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -21332,6 +22168,9 @@
       <c r="W279" t="n">
         <v>7</v>
       </c>
+      <c r="X279" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -21407,6 +22246,9 @@
       <c r="W280" t="n">
         <v>1</v>
       </c>
+      <c r="X280" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -21482,6 +22324,9 @@
       <c r="W281" t="n">
         <v>1</v>
       </c>
+      <c r="X281" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -21557,6 +22402,9 @@
       <c r="W282" t="n">
         <v>0</v>
       </c>
+      <c r="X282" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -21632,6 +22480,9 @@
       <c r="W283" t="n">
         <v>0</v>
       </c>
+      <c r="X283" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -21707,6 +22558,9 @@
       <c r="W284" t="n">
         <v>1</v>
       </c>
+      <c r="X284" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -21782,6 +22636,9 @@
       <c r="W285" t="n">
         <v>1</v>
       </c>
+      <c r="X285" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -21857,6 +22714,9 @@
       <c r="W286" t="n">
         <v>4</v>
       </c>
+      <c r="X286" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -21932,6 +22792,9 @@
       <c r="W287" t="n">
         <v>84</v>
       </c>
+      <c r="X287" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -22007,6 +22870,9 @@
       <c r="W288" t="n">
         <v>1</v>
       </c>
+      <c r="X288" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -22082,6 +22948,9 @@
       <c r="W289" t="n">
         <v>0</v>
       </c>
+      <c r="X289" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -22157,6 +23026,9 @@
       <c r="W290" t="n">
         <v>0</v>
       </c>
+      <c r="X290" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -22232,6 +23104,9 @@
       <c r="W291" t="n">
         <v>1</v>
       </c>
+      <c r="X291" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -22307,6 +23182,9 @@
       <c r="W292" t="n">
         <v>43</v>
       </c>
+      <c r="X292" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -22382,6 +23260,9 @@
       <c r="W293" t="n">
         <v>0</v>
       </c>
+      <c r="X293" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -22457,6 +23338,9 @@
       <c r="W294" t="n">
         <v>0</v>
       </c>
+      <c r="X294" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -22532,6 +23416,9 @@
       <c r="W295" t="n">
         <v>0</v>
       </c>
+      <c r="X295" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -22607,6 +23494,9 @@
       <c r="W296" t="n">
         <v>48</v>
       </c>
+      <c r="X296" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -22682,6 +23572,9 @@
       <c r="W297" t="n">
         <v>3</v>
       </c>
+      <c r="X297" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -22757,6 +23650,9 @@
       <c r="W298" t="n">
         <v>0</v>
       </c>
+      <c r="X298" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -22832,6 +23728,9 @@
       <c r="W299" t="n">
         <v>1</v>
       </c>
+      <c r="X299" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -22907,6 +23806,9 @@
       <c r="W300" t="n">
         <v>0</v>
       </c>
+      <c r="X300" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -22982,6 +23884,9 @@
       <c r="W301" t="n">
         <v>0</v>
       </c>
+      <c r="X301" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -23057,6 +23962,9 @@
       <c r="W302" t="n">
         <v>1</v>
       </c>
+      <c r="X302" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -23132,6 +24040,9 @@
       <c r="W303" t="n">
         <v>1</v>
       </c>
+      <c r="X303" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -23207,6 +24118,9 @@
       <c r="W304" t="n">
         <v>1</v>
       </c>
+      <c r="X304" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -23282,6 +24196,9 @@
       <c r="W305" t="n">
         <v>4</v>
       </c>
+      <c r="X305" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -23357,6 +24274,9 @@
       <c r="W306" t="n">
         <v>6</v>
       </c>
+      <c r="X306" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -23432,6 +24352,9 @@
       <c r="W307" t="n">
         <v>0</v>
       </c>
+      <c r="X307" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -23507,6 +24430,9 @@
       <c r="W308" t="n">
         <v>3</v>
       </c>
+      <c r="X308" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -23582,6 +24508,9 @@
       <c r="W309" t="n">
         <v>1</v>
       </c>
+      <c r="X309" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -23657,6 +24586,9 @@
       <c r="W310" t="n">
         <v>0</v>
       </c>
+      <c r="X310" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -23732,6 +24664,9 @@
       <c r="W311" t="n">
         <v>3</v>
       </c>
+      <c r="X311" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -23807,6 +24742,9 @@
       <c r="W312" t="n">
         <v>0</v>
       </c>
+      <c r="X312" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -23882,6 +24820,9 @@
       <c r="W313" t="n">
         <v>0</v>
       </c>
+      <c r="X313" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -23957,6 +24898,9 @@
       <c r="W314" t="n">
         <v>1</v>
       </c>
+      <c r="X314" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -24032,6 +24976,9 @@
       <c r="W315" t="n">
         <v>3</v>
       </c>
+      <c r="X315" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -24107,6 +25054,9 @@
       <c r="W316" t="n">
         <v>0</v>
       </c>
+      <c r="X316" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -24182,6 +25132,9 @@
       <c r="W317" t="n">
         <v>1</v>
       </c>
+      <c r="X317" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -24257,6 +25210,9 @@
       <c r="W318" t="n">
         <v>10</v>
       </c>
+      <c r="X318" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -24332,6 +25288,9 @@
       <c r="W319" t="n">
         <v>1</v>
       </c>
+      <c r="X319" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -24407,6 +25366,9 @@
       <c r="W320" t="n">
         <v>0</v>
       </c>
+      <c r="X320" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -24482,6 +25444,9 @@
       <c r="W321" t="n">
         <v>3</v>
       </c>
+      <c r="X321" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -24557,6 +25522,9 @@
       <c r="W322" t="n">
         <v>3</v>
       </c>
+      <c r="X322" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -24632,6 +25600,9 @@
       <c r="W323" t="n">
         <v>0</v>
       </c>
+      <c r="X323" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -24707,6 +25678,9 @@
       <c r="W324" t="n">
         <v>0</v>
       </c>
+      <c r="X324" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -24782,6 +25756,9 @@
       <c r="W325" t="n">
         <v>3</v>
       </c>
+      <c r="X325" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -24857,6 +25834,9 @@
       <c r="W326" t="n">
         <v>3</v>
       </c>
+      <c r="X326" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -24932,6 +25912,9 @@
       <c r="W327" t="n">
         <v>1</v>
       </c>
+      <c r="X327" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -25007,6 +25990,9 @@
       <c r="W328" t="n">
         <v>0</v>
       </c>
+      <c r="X328" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -25082,6 +26068,9 @@
       <c r="W329" t="n">
         <v>0</v>
       </c>
+      <c r="X329" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -25157,6 +26146,9 @@
       <c r="W330" t="n">
         <v>0</v>
       </c>
+      <c r="X330" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -25232,6 +26224,9 @@
       <c r="W331" t="n">
         <v>1</v>
       </c>
+      <c r="X331" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -25307,6 +26302,9 @@
       <c r="W332" t="n">
         <v>0</v>
       </c>
+      <c r="X332" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -25382,6 +26380,9 @@
       <c r="W333" t="n">
         <v>3</v>
       </c>
+      <c r="X333" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -25457,6 +26458,9 @@
       <c r="W334" t="n">
         <v>0</v>
       </c>
+      <c r="X334" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -25532,6 +26536,9 @@
       <c r="W335" t="n">
         <v>5</v>
       </c>
+      <c r="X335" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -25607,6 +26614,9 @@
       <c r="W336" t="n">
         <v>0</v>
       </c>
+      <c r="X336" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -25682,6 +26692,9 @@
       <c r="W337" t="n">
         <v>3</v>
       </c>
+      <c r="X337" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -25757,6 +26770,9 @@
       <c r="W338" t="n">
         <v>0</v>
       </c>
+      <c r="X338" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -25832,6 +26848,9 @@
       <c r="W339" t="n">
         <v>0</v>
       </c>
+      <c r="X339" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -25907,6 +26926,9 @@
       <c r="W340" t="n">
         <v>2</v>
       </c>
+      <c r="X340" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -25982,6 +27004,9 @@
       <c r="W341" t="n">
         <v>0</v>
       </c>
+      <c r="X341" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -26057,6 +27082,9 @@
       <c r="W342" t="n">
         <v>1</v>
       </c>
+      <c r="X342" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -26132,6 +27160,9 @@
       <c r="W343" t="n">
         <v>2</v>
       </c>
+      <c r="X343" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -26207,6 +27238,9 @@
       <c r="W344" t="n">
         <v>1</v>
       </c>
+      <c r="X344" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -26282,6 +27316,9 @@
       <c r="W345" t="n">
         <v>1</v>
       </c>
+      <c r="X345" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -26357,6 +27394,9 @@
       <c r="W346" t="n">
         <v>2</v>
       </c>
+      <c r="X346" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -26432,6 +27472,9 @@
       <c r="W347" t="n">
         <v>8</v>
       </c>
+      <c r="X347" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -26507,6 +27550,9 @@
       <c r="W348" t="n">
         <v>0</v>
       </c>
+      <c r="X348" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -26582,6 +27628,9 @@
       <c r="W349" t="n">
         <v>0</v>
       </c>
+      <c r="X349" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -26657,6 +27706,9 @@
       <c r="W350" t="n">
         <v>0</v>
       </c>
+      <c r="X350" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -26732,6 +27784,9 @@
       <c r="W351" t="n">
         <v>0</v>
       </c>
+      <c r="X351" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -26807,6 +27862,9 @@
       <c r="W352" t="n">
         <v>3</v>
       </c>
+      <c r="X352" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -26882,6 +27940,9 @@
       <c r="W353" t="n">
         <v>0</v>
       </c>
+      <c r="X353" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -26957,6 +28018,9 @@
       <c r="W354" t="n">
         <v>2</v>
       </c>
+      <c r="X354" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -27032,6 +28096,9 @@
       <c r="W355" t="n">
         <v>3</v>
       </c>
+      <c r="X355" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -27106,6 +28173,9 @@
       </c>
       <c r="W356" t="n">
         <v>6</v>
+      </c>
+      <c r="X356" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
22-03 update + new data for number in deaths and hospitalized in the Netherlands
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_city.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC356"/>
+  <dimension ref="A1:AD356"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,11 @@
           <t>21-03-2020</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>22-03-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -607,6 +612,9 @@
       <c r="AC2" t="n">
         <v>44</v>
       </c>
+      <c r="AD2" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -702,6 +710,9 @@
       <c r="AC3" t="n">
         <v>45</v>
       </c>
+      <c r="AD3" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -797,6 +808,9 @@
       <c r="AC4" t="n">
         <v>0</v>
       </c>
+      <c r="AD4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -892,6 +906,9 @@
       <c r="AC5" t="n">
         <v>5</v>
       </c>
+      <c r="AD5" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -987,6 +1004,9 @@
       <c r="AC6" t="n">
         <v>1</v>
       </c>
+      <c r="AD6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1082,6 +1102,9 @@
       <c r="AC7" t="n">
         <v>0</v>
       </c>
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1177,6 +1200,9 @@
       <c r="AC8" t="n">
         <v>3</v>
       </c>
+      <c r="AD8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1272,6 +1298,9 @@
       <c r="AC9" t="n">
         <v>8</v>
       </c>
+      <c r="AD9" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1367,6 +1396,9 @@
       <c r="AC10" t="n">
         <v>11</v>
       </c>
+      <c r="AD10" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1462,6 +1494,9 @@
       <c r="AC11" t="n">
         <v>4</v>
       </c>
+      <c r="AD11" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1557,6 +1592,9 @@
       <c r="AC12" t="n">
         <v>11</v>
       </c>
+      <c r="AD12" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1652,6 +1690,9 @@
       <c r="AC13" t="n">
         <v>15</v>
       </c>
+      <c r="AD13" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1747,6 +1788,9 @@
       <c r="AC14" t="n">
         <v>7</v>
       </c>
+      <c r="AD14" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1842,6 +1886,9 @@
       <c r="AC15" t="n">
         <v>22</v>
       </c>
+      <c r="AD15" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1937,6 +1984,9 @@
       <c r="AC16" t="n">
         <v>0</v>
       </c>
+      <c r="AD16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2032,6 +2082,9 @@
       <c r="AC17" t="n">
         <v>37</v>
       </c>
+      <c r="AD17" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2127,6 +2180,9 @@
       <c r="AC18" t="n">
         <v>26</v>
       </c>
+      <c r="AD18" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2222,6 +2278,9 @@
       <c r="AC19" t="n">
         <v>161</v>
       </c>
+      <c r="AD19" t="n">
+        <v>188</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2317,6 +2376,9 @@
       <c r="AC20" t="n">
         <v>16</v>
       </c>
+      <c r="AD20" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2410,6 +2472,9 @@
         <v>0</v>
       </c>
       <c r="AC21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2507,6 +2572,9 @@
       <c r="AC22" t="n">
         <v>15</v>
       </c>
+      <c r="AD22" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2602,6 +2670,9 @@
       <c r="AC23" t="n">
         <v>1</v>
       </c>
+      <c r="AD23" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2697,6 +2768,9 @@
       <c r="AC24" t="n">
         <v>5</v>
       </c>
+      <c r="AD24" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2792,6 +2866,9 @@
       <c r="AC25" t="n">
         <v>1</v>
       </c>
+      <c r="AD25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2887,6 +2964,9 @@
       <c r="AC26" t="n">
         <v>1</v>
       </c>
+      <c r="AD26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2982,6 +3062,9 @@
       <c r="AC27" t="n">
         <v>9</v>
       </c>
+      <c r="AD27" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -3077,6 +3160,9 @@
       <c r="AC28" t="n">
         <v>8</v>
       </c>
+      <c r="AD28" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -3172,6 +3258,9 @@
       <c r="AC29" t="n">
         <v>5</v>
       </c>
+      <c r="AD29" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -3267,6 +3356,9 @@
       <c r="AC30" t="n">
         <v>19</v>
       </c>
+      <c r="AD30" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -3362,6 +3454,9 @@
       <c r="AC31" t="n">
         <v>0</v>
       </c>
+      <c r="AD31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -3457,6 +3552,9 @@
       <c r="AC32" t="n">
         <v>3</v>
       </c>
+      <c r="AD32" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -3552,6 +3650,9 @@
       <c r="AC33" t="n">
         <v>25</v>
       </c>
+      <c r="AD33" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -3647,6 +3748,9 @@
       <c r="AC34" t="n">
         <v>1</v>
       </c>
+      <c r="AD34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3742,6 +3846,9 @@
       <c r="AC35" t="n">
         <v>1</v>
       </c>
+      <c r="AD35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3837,6 +3944,9 @@
       <c r="AC36" t="n">
         <v>6</v>
       </c>
+      <c r="AD36" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3932,6 +4042,9 @@
       <c r="AC37" t="n">
         <v>9</v>
       </c>
+      <c r="AD37" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -4027,6 +4140,9 @@
       <c r="AC38" t="n">
         <v>1</v>
       </c>
+      <c r="AD38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -4122,6 +4238,9 @@
       <c r="AC39" t="n">
         <v>41</v>
       </c>
+      <c r="AD39" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -4217,6 +4336,9 @@
       <c r="AC40" t="n">
         <v>11</v>
       </c>
+      <c r="AD40" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -4312,6 +4434,9 @@
       <c r="AC41" t="n">
         <v>9</v>
       </c>
+      <c r="AD41" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -4407,6 +4532,9 @@
       <c r="AC42" t="n">
         <v>6</v>
       </c>
+      <c r="AD42" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -4502,6 +4630,9 @@
       <c r="AC43" t="n">
         <v>7</v>
       </c>
+      <c r="AD43" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -4597,6 +4728,9 @@
       <c r="AC44" t="n">
         <v>4</v>
       </c>
+      <c r="AD44" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -4692,6 +4826,9 @@
       <c r="AC45" t="n">
         <v>8</v>
       </c>
+      <c r="AD45" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4787,6 +4924,9 @@
       <c r="AC46" t="n">
         <v>3</v>
       </c>
+      <c r="AD46" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -4882,6 +5022,9 @@
       <c r="AC47" t="n">
         <v>32</v>
       </c>
+      <c r="AD47" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -4977,6 +5120,9 @@
       <c r="AC48" t="n">
         <v>0</v>
       </c>
+      <c r="AD48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -5072,6 +5218,9 @@
       <c r="AC49" t="n">
         <v>4</v>
       </c>
+      <c r="AD49" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -5167,6 +5316,9 @@
       <c r="AC50" t="n">
         <v>3</v>
       </c>
+      <c r="AD50" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -5262,6 +5414,9 @@
       <c r="AC51" t="n">
         <v>6</v>
       </c>
+      <c r="AD51" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -5357,6 +5512,9 @@
       <c r="AC52" t="n">
         <v>11</v>
       </c>
+      <c r="AD52" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -5452,6 +5610,9 @@
       <c r="AC53" t="n">
         <v>133</v>
       </c>
+      <c r="AD53" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -5547,6 +5708,9 @@
       <c r="AC54" t="n">
         <v>1</v>
       </c>
+      <c r="AD54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -5642,6 +5806,9 @@
       <c r="AC55" t="n">
         <v>6</v>
       </c>
+      <c r="AD55" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -5737,6 +5904,9 @@
       <c r="AC56" t="n">
         <v>1</v>
       </c>
+      <c r="AD56" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -5832,6 +6002,9 @@
       <c r="AC57" t="n">
         <v>6</v>
       </c>
+      <c r="AD57" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -5927,6 +6100,9 @@
       <c r="AC58" t="n">
         <v>3</v>
       </c>
+      <c r="AD58" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -6022,6 +6198,9 @@
       <c r="AC59" t="n">
         <v>0</v>
       </c>
+      <c r="AD59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -6117,6 +6296,9 @@
       <c r="AC60" t="n">
         <v>5</v>
       </c>
+      <c r="AD60" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -6212,6 +6394,9 @@
       <c r="AC61" t="n">
         <v>3</v>
       </c>
+      <c r="AD61" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -6307,6 +6492,9 @@
       <c r="AC62" t="n">
         <v>7</v>
       </c>
+      <c r="AD62" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -6402,6 +6590,9 @@
       <c r="AC63" t="n">
         <v>14</v>
       </c>
+      <c r="AD63" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -6497,6 +6688,9 @@
       <c r="AC64" t="n">
         <v>11</v>
       </c>
+      <c r="AD64" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -6592,6 +6786,9 @@
       <c r="AC65" t="n">
         <v>4</v>
       </c>
+      <c r="AD65" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -6687,6 +6884,9 @@
       <c r="AC66" t="n">
         <v>5</v>
       </c>
+      <c r="AD66" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -6782,6 +6982,9 @@
       <c r="AC67" t="n">
         <v>5</v>
       </c>
+      <c r="AD67" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -6877,6 +7080,9 @@
       <c r="AC68" t="n">
         <v>0</v>
       </c>
+      <c r="AD68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -6972,6 +7178,9 @@
       <c r="AC69" t="n">
         <v>19</v>
       </c>
+      <c r="AD69" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -7067,6 +7276,9 @@
       <c r="AC70" t="n">
         <v>8</v>
       </c>
+      <c r="AD70" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -7162,6 +7374,9 @@
       <c r="AC71" t="n">
         <v>3</v>
       </c>
+      <c r="AD71" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -7257,6 +7472,9 @@
       <c r="AC72" t="n">
         <v>3</v>
       </c>
+      <c r="AD72" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -7352,6 +7570,9 @@
       <c r="AC73" t="n">
         <v>11</v>
       </c>
+      <c r="AD73" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -7447,6 +7668,9 @@
       <c r="AC74" t="n">
         <v>0</v>
       </c>
+      <c r="AD74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -7542,6 +7766,9 @@
       <c r="AC75" t="n">
         <v>3</v>
       </c>
+      <c r="AD75" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -7637,6 +7864,9 @@
       <c r="AC76" t="n">
         <v>19</v>
       </c>
+      <c r="AD76" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -7732,6 +7962,9 @@
       <c r="AC77" t="n">
         <v>16</v>
       </c>
+      <c r="AD77" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -7827,6 +8060,9 @@
       <c r="AC78" t="n">
         <v>3</v>
       </c>
+      <c r="AD78" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -7922,6 +8158,9 @@
       <c r="AC79" t="n">
         <v>13</v>
       </c>
+      <c r="AD79" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -8017,6 +8256,9 @@
       <c r="AC80" t="n">
         <v>3</v>
       </c>
+      <c r="AD80" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -8112,6 +8354,9 @@
       <c r="AC81" t="n">
         <v>5</v>
       </c>
+      <c r="AD81" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -8207,6 +8452,9 @@
       <c r="AC82" t="n">
         <v>2</v>
       </c>
+      <c r="AD82" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -8302,6 +8550,9 @@
       <c r="AC83" t="n">
         <v>12</v>
       </c>
+      <c r="AD83" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -8397,6 +8648,9 @@
       <c r="AC84" t="n">
         <v>2</v>
       </c>
+      <c r="AD84" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -8492,6 +8746,9 @@
       <c r="AC85" t="n">
         <v>14</v>
       </c>
+      <c r="AD85" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -8587,6 +8844,9 @@
       <c r="AC86" t="n">
         <v>11</v>
       </c>
+      <c r="AD86" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -8682,6 +8942,9 @@
       <c r="AC87" t="n">
         <v>5</v>
       </c>
+      <c r="AD87" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -8777,6 +9040,9 @@
       <c r="AC88" t="n">
         <v>2</v>
       </c>
+      <c r="AD88" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -8872,6 +9138,9 @@
       <c r="AC89" t="n">
         <v>11</v>
       </c>
+      <c r="AD89" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -8967,6 +9236,9 @@
       <c r="AC90" t="n">
         <v>4</v>
       </c>
+      <c r="AD90" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -9062,6 +9334,9 @@
       <c r="AC91" t="n">
         <v>13</v>
       </c>
+      <c r="AD91" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -9157,6 +9432,9 @@
       <c r="AC92" t="n">
         <v>1</v>
       </c>
+      <c r="AD92" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -9252,6 +9530,9 @@
       <c r="AC93" t="n">
         <v>7</v>
       </c>
+      <c r="AD93" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -9347,6 +9628,9 @@
       <c r="AC94" t="n">
         <v>6</v>
       </c>
+      <c r="AD94" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -9442,6 +9726,9 @@
       <c r="AC95" t="n">
         <v>35</v>
       </c>
+      <c r="AD95" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -9537,6 +9824,9 @@
       <c r="AC96" t="n">
         <v>2</v>
       </c>
+      <c r="AD96" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -9632,6 +9922,9 @@
       <c r="AC97" t="n">
         <v>4</v>
       </c>
+      <c r="AD97" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -9727,6 +10020,9 @@
       <c r="AC98" t="n">
         <v>6</v>
       </c>
+      <c r="AD98" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -9822,6 +10118,9 @@
       <c r="AC99" t="n">
         <v>16</v>
       </c>
+      <c r="AD99" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -9917,6 +10216,9 @@
       <c r="AC100" t="n">
         <v>6</v>
       </c>
+      <c r="AD100" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -10012,6 +10314,9 @@
       <c r="AC101" t="n">
         <v>11</v>
       </c>
+      <c r="AD101" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -10107,6 +10412,9 @@
       <c r="AC102" t="n">
         <v>18</v>
       </c>
+      <c r="AD102" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -10202,6 +10510,9 @@
       <c r="AC103" t="n">
         <v>7</v>
       </c>
+      <c r="AD103" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -10297,6 +10608,9 @@
       <c r="AC104" t="n">
         <v>6</v>
       </c>
+      <c r="AD104" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -10392,6 +10706,9 @@
       <c r="AC105" t="n">
         <v>42</v>
       </c>
+      <c r="AD105" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -10487,6 +10804,9 @@
       <c r="AC106" t="n">
         <v>5</v>
       </c>
+      <c r="AD106" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -10582,6 +10902,9 @@
       <c r="AC107" t="n">
         <v>7</v>
       </c>
+      <c r="AD107" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -10677,6 +11000,9 @@
       <c r="AC108" t="n">
         <v>16</v>
       </c>
+      <c r="AD108" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -10772,6 +11098,9 @@
       <c r="AC109" t="n">
         <v>3</v>
       </c>
+      <c r="AD109" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -10867,6 +11196,9 @@
       <c r="AC110" t="n">
         <v>12</v>
       </c>
+      <c r="AD110" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -10962,6 +11294,9 @@
       <c r="AC111" t="n">
         <v>11</v>
       </c>
+      <c r="AD111" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -11057,6 +11392,9 @@
       <c r="AC112" t="n">
         <v>0</v>
       </c>
+      <c r="AD112" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -11152,6 +11490,9 @@
       <c r="AC113" t="n">
         <v>12</v>
       </c>
+      <c r="AD113" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -11247,6 +11588,9 @@
       <c r="AC114" t="n">
         <v>6</v>
       </c>
+      <c r="AD114" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -11342,6 +11686,9 @@
       <c r="AC115" t="n">
         <v>39</v>
       </c>
+      <c r="AD115" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -11437,6 +11784,9 @@
       <c r="AC116" t="n">
         <v>2</v>
       </c>
+      <c r="AD116" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -11532,6 +11882,9 @@
       <c r="AC117" t="n">
         <v>1</v>
       </c>
+      <c r="AD117" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -11627,6 +11980,9 @@
       <c r="AC118" t="n">
         <v>10</v>
       </c>
+      <c r="AD118" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -11722,6 +12078,9 @@
       <c r="AC119" t="n">
         <v>25</v>
       </c>
+      <c r="AD119" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -11817,6 +12176,9 @@
       <c r="AC120" t="n">
         <v>12</v>
       </c>
+      <c r="AD120" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -11912,6 +12274,9 @@
       <c r="AC121" t="n">
         <v>5</v>
       </c>
+      <c r="AD121" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -12007,6 +12372,9 @@
       <c r="AC122" t="n">
         <v>3</v>
       </c>
+      <c r="AD122" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -12102,6 +12470,9 @@
       <c r="AC123" t="n">
         <v>5</v>
       </c>
+      <c r="AD123" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -12197,6 +12568,9 @@
       <c r="AC124" t="n">
         <v>6</v>
       </c>
+      <c r="AD124" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -12292,6 +12666,9 @@
       <c r="AC125" t="n">
         <v>3</v>
       </c>
+      <c r="AD125" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -12387,6 +12764,9 @@
       <c r="AC126" t="n">
         <v>1</v>
       </c>
+      <c r="AD126" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -12482,6 +12862,9 @@
       <c r="AC127" t="n">
         <v>5</v>
       </c>
+      <c r="AD127" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -12577,6 +12960,9 @@
       <c r="AC128" t="n">
         <v>11</v>
       </c>
+      <c r="AD128" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -12672,6 +13058,9 @@
       <c r="AC129" t="n">
         <v>9</v>
       </c>
+      <c r="AD129" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -12767,6 +13156,9 @@
       <c r="AC130" t="n">
         <v>2</v>
       </c>
+      <c r="AD130" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -12862,6 +13254,9 @@
       <c r="AC131" t="n">
         <v>5</v>
       </c>
+      <c r="AD131" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -12957,6 +13352,9 @@
       <c r="AC132" t="n">
         <v>19</v>
       </c>
+      <c r="AD132" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -13052,6 +13450,9 @@
       <c r="AC133" t="n">
         <v>4</v>
       </c>
+      <c r="AD133" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -13147,6 +13548,9 @@
       <c r="AC134" t="n">
         <v>4</v>
       </c>
+      <c r="AD134" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -13242,6 +13646,9 @@
       <c r="AC135" t="n">
         <v>3</v>
       </c>
+      <c r="AD135" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -13337,6 +13744,9 @@
       <c r="AC136" t="n">
         <v>4</v>
       </c>
+      <c r="AD136" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -13432,6 +13842,9 @@
       <c r="AC137" t="n">
         <v>32</v>
       </c>
+      <c r="AD137" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -13527,6 +13940,9 @@
       <c r="AC138" t="n">
         <v>0</v>
       </c>
+      <c r="AD138" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -13622,6 +14038,9 @@
       <c r="AC139" t="n">
         <v>13</v>
       </c>
+      <c r="AD139" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -13717,6 +14136,9 @@
       <c r="AC140" t="n">
         <v>0</v>
       </c>
+      <c r="AD140" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -13812,6 +14234,9 @@
       <c r="AC141" t="n">
         <v>7</v>
       </c>
+      <c r="AD141" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -13907,6 +14332,9 @@
       <c r="AC142" t="n">
         <v>11</v>
       </c>
+      <c r="AD142" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -14002,6 +14430,9 @@
       <c r="AC143" t="n">
         <v>2</v>
       </c>
+      <c r="AD143" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -14097,6 +14528,9 @@
       <c r="AC144" t="n">
         <v>5</v>
       </c>
+      <c r="AD144" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -14192,6 +14626,9 @@
       <c r="AC145" t="n">
         <v>7</v>
       </c>
+      <c r="AD145" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -14287,6 +14724,9 @@
       <c r="AC146" t="n">
         <v>17</v>
       </c>
+      <c r="AD146" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -14382,6 +14822,9 @@
       <c r="AC147" t="n">
         <v>4</v>
       </c>
+      <c r="AD147" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -14477,6 +14920,9 @@
       <c r="AC148" t="n">
         <v>6</v>
       </c>
+      <c r="AD148" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -14572,6 +15018,9 @@
       <c r="AC149" t="n">
         <v>5</v>
       </c>
+      <c r="AD149" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -14667,6 +15116,9 @@
       <c r="AC150" t="n">
         <v>8</v>
       </c>
+      <c r="AD150" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -14762,6 +15214,9 @@
       <c r="AC151" t="n">
         <v>13</v>
       </c>
+      <c r="AD151" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -14857,6 +15312,9 @@
       <c r="AC152" t="n">
         <v>19</v>
       </c>
+      <c r="AD152" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -14952,6 +15410,9 @@
       <c r="AC153" t="n">
         <v>3</v>
       </c>
+      <c r="AD153" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -15047,6 +15508,9 @@
       <c r="AC154" t="n">
         <v>0</v>
       </c>
+      <c r="AD154" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -15142,6 +15606,9 @@
       <c r="AC155" t="n">
         <v>11</v>
       </c>
+      <c r="AD155" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -15237,6 +15704,9 @@
       <c r="AC156" t="n">
         <v>1</v>
       </c>
+      <c r="AD156" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -15332,6 +15802,9 @@
       <c r="AC157" t="n">
         <v>12</v>
       </c>
+      <c r="AD157" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -15427,6 +15900,9 @@
       <c r="AC158" t="n">
         <v>2</v>
       </c>
+      <c r="AD158" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -15522,6 +15998,9 @@
       <c r="AC159" t="n">
         <v>5</v>
       </c>
+      <c r="AD159" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -15617,6 +16096,9 @@
       <c r="AC160" t="n">
         <v>6</v>
       </c>
+      <c r="AD160" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -15712,6 +16194,9 @@
       <c r="AC161" t="n">
         <v>1</v>
       </c>
+      <c r="AD161" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -15807,6 +16292,9 @@
       <c r="AC162" t="n">
         <v>2</v>
       </c>
+      <c r="AD162" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -15902,6 +16390,9 @@
       <c r="AC163" t="n">
         <v>9</v>
       </c>
+      <c r="AD163" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -15997,6 +16488,9 @@
       <c r="AC164" t="n">
         <v>8</v>
       </c>
+      <c r="AD164" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -16092,6 +16586,9 @@
       <c r="AC165" t="n">
         <v>20</v>
       </c>
+      <c r="AD165" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -16187,6 +16684,9 @@
       <c r="AC166" t="n">
         <v>9</v>
       </c>
+      <c r="AD166" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -16282,6 +16782,9 @@
       <c r="AC167" t="n">
         <v>4</v>
       </c>
+      <c r="AD167" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -16377,6 +16880,9 @@
       <c r="AC168" t="n">
         <v>4</v>
       </c>
+      <c r="AD168" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -16472,6 +16978,9 @@
       <c r="AC169" t="n">
         <v>16</v>
       </c>
+      <c r="AD169" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -16567,6 +17076,9 @@
       <c r="AC170" t="n">
         <v>0</v>
       </c>
+      <c r="AD170" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -16662,6 +17174,9 @@
       <c r="AC171" t="n">
         <v>8</v>
       </c>
+      <c r="AD171" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -16757,6 +17272,9 @@
       <c r="AC172" t="n">
         <v>16</v>
       </c>
+      <c r="AD172" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -16852,6 +17370,9 @@
       <c r="AC173" t="n">
         <v>2</v>
       </c>
+      <c r="AD173" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -16947,6 +17468,9 @@
       <c r="AC174" t="n">
         <v>9</v>
       </c>
+      <c r="AD174" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -17042,6 +17566,9 @@
       <c r="AC175" t="n">
         <v>15</v>
       </c>
+      <c r="AD175" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -17137,6 +17664,9 @@
       <c r="AC176" t="n">
         <v>20</v>
       </c>
+      <c r="AD176" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -17232,6 +17762,9 @@
       <c r="AC177" t="n">
         <v>6</v>
       </c>
+      <c r="AD177" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -17327,6 +17860,9 @@
       <c r="AC178" t="n">
         <v>6</v>
       </c>
+      <c r="AD178" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -17422,6 +17958,9 @@
       <c r="AC179" t="n">
         <v>0</v>
       </c>
+      <c r="AD179" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -17517,6 +18056,9 @@
       <c r="AC180" t="n">
         <v>2</v>
       </c>
+      <c r="AD180" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -17612,6 +18154,9 @@
       <c r="AC181" t="n">
         <v>14</v>
       </c>
+      <c r="AD181" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -17707,6 +18252,9 @@
       <c r="AC182" t="n">
         <v>4</v>
       </c>
+      <c r="AD182" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -17802,6 +18350,9 @@
       <c r="AC183" t="n">
         <v>0</v>
       </c>
+      <c r="AD183" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -17897,6 +18448,9 @@
       <c r="AC184" t="n">
         <v>1</v>
       </c>
+      <c r="AD184" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -17992,6 +18546,9 @@
       <c r="AC185" t="n">
         <v>2</v>
       </c>
+      <c r="AD185" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -18087,6 +18644,9 @@
       <c r="AC186" t="n">
         <v>7</v>
       </c>
+      <c r="AD186" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -18182,6 +18742,9 @@
       <c r="AC187" t="n">
         <v>3</v>
       </c>
+      <c r="AD187" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -18277,6 +18840,9 @@
       <c r="AC188" t="n">
         <v>57</v>
       </c>
+      <c r="AD188" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -18372,6 +18938,9 @@
       <c r="AC189" t="n">
         <v>1</v>
       </c>
+      <c r="AD189" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -18467,6 +19036,9 @@
       <c r="AC190" t="n">
         <v>2</v>
       </c>
+      <c r="AD190" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -18562,6 +19134,9 @@
       <c r="AC191" t="n">
         <v>95</v>
       </c>
+      <c r="AD191" t="n">
+        <v>119</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -18657,6 +19232,9 @@
       <c r="AC192" t="n">
         <v>1</v>
       </c>
+      <c r="AD192" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -18752,6 +19330,9 @@
       <c r="AC193" t="n">
         <v>4</v>
       </c>
+      <c r="AD193" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -18847,6 +19428,9 @@
       <c r="AC194" t="n">
         <v>2</v>
       </c>
+      <c r="AD194" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -18942,6 +19526,9 @@
       <c r="AC195" t="n">
         <v>1</v>
       </c>
+      <c r="AD195" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -19037,6 +19624,9 @@
       <c r="AC196" t="n">
         <v>2</v>
       </c>
+      <c r="AD196" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -19132,6 +19722,9 @@
       <c r="AC197" t="n">
         <v>2</v>
       </c>
+      <c r="AD197" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -19227,6 +19820,9 @@
       <c r="AC198" t="n">
         <v>3</v>
       </c>
+      <c r="AD198" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -19322,6 +19918,9 @@
       <c r="AC199" t="n">
         <v>11</v>
       </c>
+      <c r="AD199" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -19417,6 +20016,9 @@
       <c r="AC200" t="n">
         <v>1</v>
       </c>
+      <c r="AD200" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -19512,6 +20114,9 @@
       <c r="AC201" t="n">
         <v>0</v>
       </c>
+      <c r="AD201" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -19607,6 +20212,9 @@
       <c r="AC202" t="n">
         <v>1</v>
       </c>
+      <c r="AD202" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -19702,6 +20310,9 @@
       <c r="AC203" t="n">
         <v>5</v>
       </c>
+      <c r="AD203" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -19797,6 +20408,9 @@
       <c r="AC204" t="n">
         <v>7</v>
       </c>
+      <c r="AD204" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -19892,6 +20506,9 @@
       <c r="AC205" t="n">
         <v>9</v>
       </c>
+      <c r="AD205" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -19987,6 +20604,9 @@
       <c r="AC206" t="n">
         <v>2</v>
       </c>
+      <c r="AD206" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -20082,6 +20702,9 @@
       <c r="AC207" t="n">
         <v>4</v>
       </c>
+      <c r="AD207" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -20177,6 +20800,9 @@
       <c r="AC208" t="n">
         <v>60</v>
       </c>
+      <c r="AD208" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -20272,6 +20898,9 @@
       <c r="AC209" t="n">
         <v>12</v>
       </c>
+      <c r="AD209" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -20367,6 +20996,9 @@
       <c r="AC210" t="n">
         <v>1</v>
       </c>
+      <c r="AD210" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -20462,6 +21094,9 @@
       <c r="AC211" t="n">
         <v>0</v>
       </c>
+      <c r="AD211" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -20557,6 +21192,9 @@
       <c r="AC212" t="n">
         <v>1</v>
       </c>
+      <c r="AD212" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -20652,6 +21290,9 @@
       <c r="AC213" t="n">
         <v>3</v>
       </c>
+      <c r="AD213" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -20747,6 +21388,9 @@
       <c r="AC214" t="n">
         <v>3</v>
       </c>
+      <c r="AD214" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -20842,6 +21486,9 @@
       <c r="AC215" t="n">
         <v>1</v>
       </c>
+      <c r="AD215" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -20937,6 +21584,9 @@
       <c r="AC216" t="n">
         <v>9</v>
       </c>
+      <c r="AD216" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -21032,6 +21682,9 @@
       <c r="AC217" t="n">
         <v>7</v>
       </c>
+      <c r="AD217" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -21127,6 +21780,9 @@
       <c r="AC218" t="n">
         <v>1</v>
       </c>
+      <c r="AD218" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -21222,6 +21878,9 @@
       <c r="AC219" t="n">
         <v>15</v>
       </c>
+      <c r="AD219" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -21317,6 +21976,9 @@
       <c r="AC220" t="n">
         <v>0</v>
       </c>
+      <c r="AD220" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -21412,6 +22074,9 @@
       <c r="AC221" t="n">
         <v>6</v>
       </c>
+      <c r="AD221" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -21507,6 +22172,9 @@
       <c r="AC222" t="n">
         <v>6</v>
       </c>
+      <c r="AD222" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -21602,6 +22270,9 @@
       <c r="AC223" t="n">
         <v>2</v>
       </c>
+      <c r="AD223" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -21697,6 +22368,9 @@
       <c r="AC224" t="n">
         <v>4</v>
       </c>
+      <c r="AD224" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -21792,6 +22466,9 @@
       <c r="AC225" t="n">
         <v>2</v>
       </c>
+      <c r="AD225" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -21887,6 +22564,9 @@
       <c r="AC226" t="n">
         <v>13</v>
       </c>
+      <c r="AD226" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -21982,6 +22662,9 @@
       <c r="AC227" t="n">
         <v>0</v>
       </c>
+      <c r="AD227" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -22077,6 +22760,9 @@
       <c r="AC228" t="n">
         <v>3</v>
       </c>
+      <c r="AD228" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -22172,6 +22858,9 @@
       <c r="AC229" t="n">
         <v>0</v>
       </c>
+      <c r="AD229" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -22267,6 +22956,9 @@
       <c r="AC230" t="n">
         <v>2</v>
       </c>
+      <c r="AD230" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -22362,6 +23054,9 @@
       <c r="AC231" t="n">
         <v>44</v>
       </c>
+      <c r="AD231" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -22457,6 +23152,9 @@
       <c r="AC232" t="n">
         <v>4</v>
       </c>
+      <c r="AD232" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -22552,6 +23250,9 @@
       <c r="AC233" t="n">
         <v>4</v>
       </c>
+      <c r="AD233" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -22647,6 +23348,9 @@
       <c r="AC234" t="n">
         <v>3</v>
       </c>
+      <c r="AD234" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -22742,6 +23446,9 @@
       <c r="AC235" t="n">
         <v>20</v>
       </c>
+      <c r="AD235" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -22837,6 +23544,9 @@
       <c r="AC236" t="n">
         <v>2</v>
       </c>
+      <c r="AD236" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -22932,6 +23642,9 @@
       <c r="AC237" t="n">
         <v>63</v>
       </c>
+      <c r="AD237" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -23027,6 +23740,9 @@
       <c r="AC238" t="n">
         <v>2</v>
       </c>
+      <c r="AD238" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -23122,6 +23838,9 @@
       <c r="AC239" t="n">
         <v>11</v>
       </c>
+      <c r="AD239" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -23217,6 +23936,9 @@
       <c r="AC240" t="n">
         <v>14</v>
       </c>
+      <c r="AD240" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -23312,6 +24034,9 @@
       <c r="AC241" t="n">
         <v>3</v>
       </c>
+      <c r="AD241" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -23407,6 +24132,9 @@
       <c r="AC242" t="n">
         <v>3</v>
       </c>
+      <c r="AD242" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -23502,6 +24230,9 @@
       <c r="AC243" t="n">
         <v>5</v>
       </c>
+      <c r="AD243" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -23597,6 +24328,9 @@
       <c r="AC244" t="n">
         <v>9</v>
       </c>
+      <c r="AD244" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -23692,6 +24426,9 @@
       <c r="AC245" t="n">
         <v>0</v>
       </c>
+      <c r="AD245" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -23787,6 +24524,9 @@
       <c r="AC246" t="n">
         <v>0</v>
       </c>
+      <c r="AD246" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -23882,6 +24622,9 @@
       <c r="AC247" t="n">
         <v>7</v>
       </c>
+      <c r="AD247" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -23977,6 +24720,9 @@
       <c r="AC248" t="n">
         <v>0</v>
       </c>
+      <c r="AD248" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -24072,6 +24818,9 @@
       <c r="AC249" t="n">
         <v>4</v>
       </c>
+      <c r="AD249" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -24167,6 +24916,9 @@
       <c r="AC250" t="n">
         <v>3</v>
       </c>
+      <c r="AD250" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -24262,6 +25014,9 @@
       <c r="AC251" t="n">
         <v>4</v>
       </c>
+      <c r="AD251" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -24357,6 +25112,9 @@
       <c r="AC252" t="n">
         <v>4</v>
       </c>
+      <c r="AD252" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -24452,6 +25210,9 @@
       <c r="AC253" t="n">
         <v>18</v>
       </c>
+      <c r="AD253" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -24547,6 +25308,9 @@
       <c r="AC254" t="n">
         <v>8</v>
       </c>
+      <c r="AD254" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -24642,6 +25406,9 @@
       <c r="AC255" t="n">
         <v>120</v>
       </c>
+      <c r="AD255" t="n">
+        <v>139</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -24737,6 +25504,9 @@
       <c r="AC256" t="n">
         <v>2</v>
       </c>
+      <c r="AD256" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -24832,6 +25602,9 @@
       <c r="AC257" t="n">
         <v>6</v>
       </c>
+      <c r="AD257" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -24927,6 +25700,9 @@
       <c r="AC258" t="n">
         <v>7</v>
       </c>
+      <c r="AD258" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -25022,6 +25798,9 @@
       <c r="AC259" t="n">
         <v>0</v>
       </c>
+      <c r="AD259" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -25117,6 +25896,9 @@
       <c r="AC260" t="n">
         <v>6</v>
       </c>
+      <c r="AD260" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -25212,6 +25994,9 @@
       <c r="AC261" t="n">
         <v>0</v>
       </c>
+      <c r="AD261" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -25307,6 +26092,9 @@
       <c r="AC262" t="n">
         <v>3</v>
       </c>
+      <c r="AD262" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -25402,6 +26190,9 @@
       <c r="AC263" t="n">
         <v>5</v>
       </c>
+      <c r="AD263" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -25497,6 +26288,9 @@
       <c r="AC264" t="n">
         <v>12</v>
       </c>
+      <c r="AD264" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -25592,6 +26386,9 @@
       <c r="AC265" t="n">
         <v>12</v>
       </c>
+      <c r="AD265" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -25687,6 +26484,9 @@
       <c r="AC266" t="n">
         <v>58</v>
       </c>
+      <c r="AD266" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -25782,6 +26582,9 @@
       <c r="AC267" t="n">
         <v>3</v>
       </c>
+      <c r="AD267" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -25877,6 +26680,9 @@
       <c r="AC268" t="n">
         <v>3</v>
       </c>
+      <c r="AD268" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -25972,6 +26778,9 @@
       <c r="AC269" t="n">
         <v>3</v>
       </c>
+      <c r="AD269" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -26067,6 +26876,9 @@
       <c r="AC270" t="n">
         <v>15</v>
       </c>
+      <c r="AD270" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -26162,6 +26974,9 @@
       <c r="AC271" t="n">
         <v>5</v>
       </c>
+      <c r="AD271" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -26257,6 +27072,9 @@
       <c r="AC272" t="n">
         <v>8</v>
       </c>
+      <c r="AD272" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -26352,6 +27170,9 @@
       <c r="AC273" t="n">
         <v>0</v>
       </c>
+      <c r="AD273" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -26447,6 +27268,9 @@
       <c r="AC274" t="n">
         <v>3</v>
       </c>
+      <c r="AD274" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -26542,6 +27366,9 @@
       <c r="AC275" t="n">
         <v>5</v>
       </c>
+      <c r="AD275" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -26637,6 +27464,9 @@
       <c r="AC276" t="n">
         <v>5</v>
       </c>
+      <c r="AD276" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -26732,6 +27562,9 @@
       <c r="AC277" t="n">
         <v>3</v>
       </c>
+      <c r="AD277" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -26827,6 +27660,9 @@
       <c r="AC278" t="n">
         <v>5</v>
       </c>
+      <c r="AD278" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -26922,6 +27758,9 @@
       <c r="AC279" t="n">
         <v>10</v>
       </c>
+      <c r="AD279" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -27017,6 +27856,9 @@
       <c r="AC280" t="n">
         <v>4</v>
       </c>
+      <c r="AD280" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -27112,6 +27954,9 @@
       <c r="AC281" t="n">
         <v>5</v>
       </c>
+      <c r="AD281" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -27207,6 +28052,9 @@
       <c r="AC282" t="n">
         <v>0</v>
       </c>
+      <c r="AD282" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -27302,6 +28150,9 @@
       <c r="AC283" t="n">
         <v>3</v>
       </c>
+      <c r="AD283" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -27397,6 +28248,9 @@
       <c r="AC284" t="n">
         <v>5</v>
       </c>
+      <c r="AD284" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -27492,6 +28346,9 @@
       <c r="AC285" t="n">
         <v>7</v>
       </c>
+      <c r="AD285" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -27587,6 +28444,9 @@
       <c r="AC286" t="n">
         <v>4</v>
       </c>
+      <c r="AD286" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -27682,6 +28542,9 @@
       <c r="AC287" t="n">
         <v>154</v>
       </c>
+      <c r="AD287" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -27777,6 +28640,9 @@
       <c r="AC288" t="n">
         <v>3</v>
       </c>
+      <c r="AD288" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -27872,6 +28738,9 @@
       <c r="AC289" t="n">
         <v>1</v>
       </c>
+      <c r="AD289" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -27967,6 +28836,9 @@
       <c r="AC290" t="n">
         <v>7</v>
       </c>
+      <c r="AD290" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -28062,6 +28934,9 @@
       <c r="AC291" t="n">
         <v>1</v>
       </c>
+      <c r="AD291" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -28157,6 +29032,9 @@
       <c r="AC292" t="n">
         <v>76</v>
       </c>
+      <c r="AD292" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -28252,6 +29130,9 @@
       <c r="AC293" t="n">
         <v>2</v>
       </c>
+      <c r="AD293" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -28347,6 +29228,9 @@
       <c r="AC294" t="n">
         <v>2</v>
       </c>
+      <c r="AD294" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -28442,6 +29326,9 @@
       <c r="AC295" t="n">
         <v>6</v>
       </c>
+      <c r="AD295" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -28537,6 +29424,9 @@
       <c r="AC296" t="n">
         <v>121</v>
       </c>
+      <c r="AD296" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -28632,6 +29522,9 @@
       <c r="AC297" t="n">
         <v>8</v>
       </c>
+      <c r="AD297" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -28727,6 +29620,9 @@
       <c r="AC298" t="n">
         <v>0</v>
       </c>
+      <c r="AD298" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -28822,6 +29718,9 @@
       <c r="AC299" t="n">
         <v>4</v>
       </c>
+      <c r="AD299" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -28917,6 +29816,9 @@
       <c r="AC300" t="n">
         <v>4</v>
       </c>
+      <c r="AD300" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -29012,6 +29914,9 @@
       <c r="AC301" t="n">
         <v>0</v>
       </c>
+      <c r="AD301" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -29107,6 +30012,9 @@
       <c r="AC302" t="n">
         <v>2</v>
       </c>
+      <c r="AD302" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -29202,6 +30110,9 @@
       <c r="AC303" t="n">
         <v>5</v>
       </c>
+      <c r="AD303" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -29297,6 +30208,9 @@
       <c r="AC304" t="n">
         <v>9</v>
       </c>
+      <c r="AD304" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -29392,6 +30306,9 @@
       <c r="AC305" t="n">
         <v>8</v>
       </c>
+      <c r="AD305" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -29487,6 +30404,9 @@
       <c r="AC306" t="n">
         <v>33</v>
       </c>
+      <c r="AD306" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -29582,6 +30502,9 @@
       <c r="AC307" t="n">
         <v>8</v>
       </c>
+      <c r="AD307" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -29677,6 +30600,9 @@
       <c r="AC308" t="n">
         <v>9</v>
       </c>
+      <c r="AD308" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -29772,6 +30698,9 @@
       <c r="AC309" t="n">
         <v>12</v>
       </c>
+      <c r="AD309" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -29867,6 +30796,9 @@
       <c r="AC310" t="n">
         <v>0</v>
       </c>
+      <c r="AD310" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -29962,6 +30894,9 @@
       <c r="AC311" t="n">
         <v>6</v>
       </c>
+      <c r="AD311" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -30057,6 +30992,9 @@
       <c r="AC312" t="n">
         <v>4</v>
       </c>
+      <c r="AD312" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -30152,6 +31090,9 @@
       <c r="AC313" t="n">
         <v>2</v>
       </c>
+      <c r="AD313" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -30247,6 +31188,9 @@
       <c r="AC314" t="n">
         <v>2</v>
       </c>
+      <c r="AD314" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -30342,6 +31286,9 @@
       <c r="AC315" t="n">
         <v>11</v>
       </c>
+      <c r="AD315" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -30437,6 +31384,9 @@
       <c r="AC316" t="n">
         <v>0</v>
       </c>
+      <c r="AD316" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -30532,6 +31482,9 @@
       <c r="AC317" t="n">
         <v>2</v>
       </c>
+      <c r="AD317" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -30627,6 +31580,9 @@
       <c r="AC318" t="n">
         <v>16</v>
       </c>
+      <c r="AD318" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -30722,6 +31678,9 @@
       <c r="AC319" t="n">
         <v>4</v>
       </c>
+      <c r="AD319" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -30817,6 +31776,9 @@
       <c r="AC320" t="n">
         <v>3</v>
       </c>
+      <c r="AD320" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -30912,6 +31874,9 @@
       <c r="AC321" t="n">
         <v>5</v>
       </c>
+      <c r="AD321" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -31007,6 +31972,9 @@
       <c r="AC322" t="n">
         <v>8</v>
       </c>
+      <c r="AD322" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -31102,6 +32070,9 @@
       <c r="AC323" t="n">
         <v>7</v>
       </c>
+      <c r="AD323" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -31197,6 +32168,9 @@
       <c r="AC324" t="n">
         <v>1</v>
       </c>
+      <c r="AD324" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -31292,6 +32266,9 @@
       <c r="AC325" t="n">
         <v>12</v>
       </c>
+      <c r="AD325" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -31387,6 +32364,9 @@
       <c r="AC326" t="n">
         <v>4</v>
       </c>
+      <c r="AD326" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -31482,6 +32462,9 @@
       <c r="AC327" t="n">
         <v>3</v>
       </c>
+      <c r="AD327" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -31577,6 +32560,9 @@
       <c r="AC328" t="n">
         <v>1</v>
       </c>
+      <c r="AD328" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -31672,6 +32658,9 @@
       <c r="AC329" t="n">
         <v>1</v>
       </c>
+      <c r="AD329" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -31767,6 +32756,9 @@
       <c r="AC330" t="n">
         <v>0</v>
       </c>
+      <c r="AD330" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -31862,6 +32854,9 @@
       <c r="AC331" t="n">
         <v>11</v>
       </c>
+      <c r="AD331" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -31957,6 +32952,9 @@
       <c r="AC332" t="n">
         <v>1</v>
       </c>
+      <c r="AD332" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -32052,6 +33050,9 @@
       <c r="AC333" t="n">
         <v>3</v>
       </c>
+      <c r="AD333" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -32147,6 +33148,9 @@
       <c r="AC334" t="n">
         <v>0</v>
       </c>
+      <c r="AD334" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -32242,6 +33246,9 @@
       <c r="AC335" t="n">
         <v>17</v>
       </c>
+      <c r="AD335" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -32337,6 +33344,9 @@
       <c r="AC336" t="n">
         <v>1</v>
       </c>
+      <c r="AD336" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -32432,6 +33442,9 @@
       <c r="AC337" t="n">
         <v>6</v>
       </c>
+      <c r="AD337" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -32527,6 +33540,9 @@
       <c r="AC338" t="n">
         <v>1</v>
       </c>
+      <c r="AD338" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -32622,6 +33638,9 @@
       <c r="AC339" t="n">
         <v>0</v>
       </c>
+      <c r="AD339" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -32717,6 +33736,9 @@
       <c r="AC340" t="n">
         <v>6</v>
       </c>
+      <c r="AD340" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -32812,6 +33834,9 @@
       <c r="AC341" t="n">
         <v>1</v>
       </c>
+      <c r="AD341" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -32907,6 +33932,9 @@
       <c r="AC342" t="n">
         <v>3</v>
       </c>
+      <c r="AD342" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -33002,6 +34030,9 @@
       <c r="AC343" t="n">
         <v>9</v>
       </c>
+      <c r="AD343" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -33097,6 +34128,9 @@
       <c r="AC344" t="n">
         <v>5</v>
       </c>
+      <c r="AD344" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -33192,6 +34226,9 @@
       <c r="AC345" t="n">
         <v>2</v>
       </c>
+      <c r="AD345" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -33287,6 +34324,9 @@
       <c r="AC346" t="n">
         <v>4</v>
       </c>
+      <c r="AD346" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -33382,6 +34422,9 @@
       <c r="AC347" t="n">
         <v>17</v>
       </c>
+      <c r="AD347" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -33477,6 +34520,9 @@
       <c r="AC348" t="n">
         <v>6</v>
       </c>
+      <c r="AD348" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -33572,6 +34618,9 @@
       <c r="AC349" t="n">
         <v>4</v>
       </c>
+      <c r="AD349" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -33667,6 +34716,9 @@
       <c r="AC350" t="n">
         <v>0</v>
       </c>
+      <c r="AD350" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -33762,6 +34814,9 @@
       <c r="AC351" t="n">
         <v>1</v>
       </c>
+      <c r="AD351" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -33857,6 +34912,9 @@
       <c r="AC352" t="n">
         <v>7</v>
       </c>
+      <c r="AD352" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -33952,6 +35010,9 @@
       <c r="AC353" t="n">
         <v>4</v>
       </c>
+      <c r="AD353" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -34047,6 +35108,9 @@
       <c r="AC354" t="n">
         <v>15</v>
       </c>
+      <c r="AD354" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -34142,6 +35206,9 @@
       <c r="AC355" t="n">
         <v>6</v>
       </c>
+      <c r="AD355" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -34236,6 +35303,9 @@
       </c>
       <c r="AC356" t="n">
         <v>23</v>
+      </c>
+      <c r="AD356" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>